<commit_message>
Add numbers only that do at least exist in my 2nd collection book:
</commit_message>
<xml_diff>
--- a/botanical-collections_rvm.xlsx
+++ b/botanical-collections_rvm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/Desktop/botanical-collections/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\botanical-collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{880CD6DC-82EF-C84F-8037-84213AD20E0C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2DEAA7-8B58-4ECF-9A65-0DEACD97E065}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="botanical-collections_rvm" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4681" uniqueCount="474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4717" uniqueCount="510">
   <si>
     <t>collection_no</t>
   </si>
@@ -1442,13 +1442,121 @@
   </si>
   <si>
     <t>Taxonomic data</t>
+  </si>
+  <si>
+    <t>RVM_163</t>
+  </si>
+  <si>
+    <t>RVM_164</t>
+  </si>
+  <si>
+    <t>RVM_165</t>
+  </si>
+  <si>
+    <t>RVM_166</t>
+  </si>
+  <si>
+    <t>RVM_167</t>
+  </si>
+  <si>
+    <t>RVM_168</t>
+  </si>
+  <si>
+    <t>RVM_169</t>
+  </si>
+  <si>
+    <t>RVM_170</t>
+  </si>
+  <si>
+    <t>RVM_171</t>
+  </si>
+  <si>
+    <t>RVM_172</t>
+  </si>
+  <si>
+    <t>RVM_173</t>
+  </si>
+  <si>
+    <t>RVM_174</t>
+  </si>
+  <si>
+    <t>RVM_175</t>
+  </si>
+  <si>
+    <t>RVM_176</t>
+  </si>
+  <si>
+    <t>RVM_177</t>
+  </si>
+  <si>
+    <t>RVM_178</t>
+  </si>
+  <si>
+    <t>RVM_179</t>
+  </si>
+  <si>
+    <t>RVM_180</t>
+  </si>
+  <si>
+    <t>RVM_181</t>
+  </si>
+  <si>
+    <t>RVM_182</t>
+  </si>
+  <si>
+    <t>RVM_183</t>
+  </si>
+  <si>
+    <t>RVM_184</t>
+  </si>
+  <si>
+    <t>RVM_185</t>
+  </si>
+  <si>
+    <t>RVM_186</t>
+  </si>
+  <si>
+    <t>RVM_187</t>
+  </si>
+  <si>
+    <t>RVM_188</t>
+  </si>
+  <si>
+    <t>RVM_189</t>
+  </si>
+  <si>
+    <t>RVM_190</t>
+  </si>
+  <si>
+    <t>RVM_191</t>
+  </si>
+  <si>
+    <t>RVM_192</t>
+  </si>
+  <si>
+    <t>RVM_193</t>
+  </si>
+  <si>
+    <t>RVM_194</t>
+  </si>
+  <si>
+    <t>RVM_195</t>
+  </si>
+  <si>
+    <t>RVM_196</t>
+  </si>
+  <si>
+    <t>RVM_197</t>
+  </si>
+  <si>
+    <t>RVM_198</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2314,58 +2422,58 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK165"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AK201"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomRight" activeCell="C200" sqref="C200"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.85546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="68.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.88671875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="68.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.88671875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.140625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="29" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="52.33203125" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="157" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="42.28515625" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="144.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="167.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="42.33203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="144.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="167.88671875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="49" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="46.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="46.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.2">
       <c r="B1" s="6" t="s">
         <v>471</v>
       </c>
@@ -2408,7 +2516,7 @@
       <c r="AI1" s="2"/>
       <c r="AJ1" s="3"/>
     </row>
-    <row r="2" spans="1:37">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2521,7 +2629,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:37">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2631,7 +2739,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:37">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -2744,7 +2852,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="5" spans="1:37">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -2854,7 +2962,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:37">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
@@ -2964,7 +3072,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:37">
+    <row r="7" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
@@ -3074,7 +3182,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:37">
+    <row r="8" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
@@ -3184,7 +3292,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:37">
+    <row r="9" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
@@ -3291,7 +3399,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:37">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
@@ -3395,7 +3503,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:37">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
@@ -3505,7 +3613,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:37">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
@@ -3615,7 +3723,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:37">
+    <row r="13" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
@@ -3719,7 +3827,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="14" spans="1:37">
+    <row r="14" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
@@ -3823,7 +3931,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="15" spans="1:37">
+    <row r="15" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
@@ -3933,7 +4041,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="16" spans="1:37">
+    <row r="16" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
@@ -4043,7 +4151,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="17" spans="1:37">
+    <row r="17" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
@@ -4153,7 +4261,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:37">
+    <row r="18" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
@@ -4263,7 +4371,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:37">
+    <row r="19" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
@@ -4373,7 +4481,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:37">
+    <row r="20" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
@@ -4483,7 +4591,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:37">
+    <row r="21" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
@@ -4593,7 +4701,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:37">
+    <row r="22" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
@@ -4703,7 +4811,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:37">
+    <row r="23" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
@@ -4813,7 +4921,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:37">
+    <row r="24" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
@@ -4923,7 +5031,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:37">
+    <row r="25" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
@@ -5033,7 +5141,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="26" spans="1:37">
+    <row r="26" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
@@ -5143,7 +5251,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:37">
+    <row r="27" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
@@ -5253,7 +5361,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:37">
+    <row r="28" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
@@ -5363,7 +5471,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:37">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
@@ -5476,7 +5584,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="30" spans="1:37">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
@@ -5589,7 +5697,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="31" spans="1:37">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
@@ -5702,7 +5810,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="32" spans="1:37">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
@@ -5815,7 +5923,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="33" spans="1:37">
+    <row r="33" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
@@ -5925,7 +6033,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:37">
+    <row r="34" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
@@ -6035,7 +6143,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:37">
+    <row r="35" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
@@ -6145,7 +6253,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:37">
+    <row r="36" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
@@ -6258,7 +6366,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="37" spans="1:37">
+    <row r="37" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
@@ -6368,7 +6476,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="38" spans="1:37">
+    <row r="38" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
@@ -6478,7 +6586,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:37">
+    <row r="39" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
@@ -6588,7 +6696,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:37">
+    <row r="40" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
@@ -6698,7 +6806,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:37">
+    <row r="41" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
@@ -6811,7 +6919,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="42" spans="1:37">
+    <row r="42" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
@@ -6921,7 +7029,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:37">
+    <row r="43" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>52</v>
       </c>
@@ -7031,7 +7139,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="44" spans="1:37">
+    <row r="44" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>53</v>
       </c>
@@ -7141,7 +7249,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="45" spans="1:37">
+    <row r="45" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>91</v>
       </c>
@@ -7251,7 +7359,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="46" spans="1:37">
+    <row r="46" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>41</v>
       </c>
@@ -7361,7 +7469,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="47" spans="1:37">
+    <row r="47" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>42</v>
       </c>
@@ -7471,7 +7579,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="1:37">
+    <row r="48" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>43</v>
       </c>
@@ -7581,7 +7689,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="49" spans="1:37">
+    <row r="49" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>44</v>
       </c>
@@ -7691,7 +7799,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="50" spans="1:37">
+    <row r="50" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>45</v>
       </c>
@@ -7801,7 +7909,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="51" spans="1:37">
+    <row r="51" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>46</v>
       </c>
@@ -7911,7 +8019,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="52" spans="1:37">
+    <row r="52" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>47</v>
       </c>
@@ -8021,7 +8129,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:37">
+    <row r="53" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>48</v>
       </c>
@@ -8134,7 +8242,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="54" spans="1:37">
+    <row r="54" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>49</v>
       </c>
@@ -8247,7 +8355,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="55" spans="1:37">
+    <row r="55" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>50</v>
       </c>
@@ -8360,7 +8468,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" spans="1:37">
+    <row r="56" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>51</v>
       </c>
@@ -8473,7 +8581,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" spans="1:37">
+    <row r="57" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>54</v>
       </c>
@@ -8583,7 +8691,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:37">
+    <row r="58" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>55</v>
       </c>
@@ -8693,7 +8801,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:37">
+    <row r="59" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>56</v>
       </c>
@@ -8803,7 +8911,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="60" spans="1:37">
+    <row r="60" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>57</v>
       </c>
@@ -8913,7 +9021,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="1:37">
+    <row r="61" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>58</v>
       </c>
@@ -9023,7 +9131,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:37">
+    <row r="62" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>59</v>
       </c>
@@ -9133,7 +9241,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="63" spans="1:37">
+    <row r="63" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>60</v>
       </c>
@@ -9243,7 +9351,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="64" spans="1:37">
+    <row r="64" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>61</v>
       </c>
@@ -9353,7 +9461,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:36">
+    <row r="65" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>62</v>
       </c>
@@ -9463,7 +9571,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="66" spans="1:36">
+    <row r="66" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>63</v>
       </c>
@@ -9573,7 +9681,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="67" spans="1:36">
+    <row r="67" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>64</v>
       </c>
@@ -9683,7 +9791,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="68" spans="1:36">
+    <row r="68" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>65</v>
       </c>
@@ -9793,7 +9901,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="69" spans="1:36">
+    <row r="69" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>66</v>
       </c>
@@ -9903,7 +10011,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="70" spans="1:36">
+    <row r="70" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>67</v>
       </c>
@@ -10010,7 +10118,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="71" spans="1:36">
+    <row r="71" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>68</v>
       </c>
@@ -10117,7 +10225,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="72" spans="1:36">
+    <row r="72" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>69</v>
       </c>
@@ -10224,7 +10332,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="73" spans="1:36">
+    <row r="73" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>70</v>
       </c>
@@ -10331,7 +10439,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="74" spans="1:36">
+    <row r="74" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>71</v>
       </c>
@@ -10441,7 +10549,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="75" spans="1:36">
+    <row r="75" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>72</v>
       </c>
@@ -10551,7 +10659,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="76" spans="1:36">
+    <row r="76" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>73</v>
       </c>
@@ -10661,7 +10769,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:36">
+    <row r="77" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>74</v>
       </c>
@@ -10771,7 +10879,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="78" spans="1:36">
+    <row r="78" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>75</v>
       </c>
@@ -10881,7 +10989,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="79" spans="1:36">
+    <row r="79" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>76</v>
       </c>
@@ -10991,7 +11099,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:36">
+    <row r="80" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>77</v>
       </c>
@@ -11101,7 +11209,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="81" spans="1:37">
+    <row r="81" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>78</v>
       </c>
@@ -11211,7 +11319,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="82" spans="1:37">
+    <row r="82" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>79</v>
       </c>
@@ -11321,7 +11429,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:37">
+    <row r="83" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>80</v>
       </c>
@@ -11431,7 +11539,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:37">
+    <row r="84" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>81</v>
       </c>
@@ -11541,7 +11649,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="85" spans="1:37">
+    <row r="85" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>82</v>
       </c>
@@ -11651,7 +11759,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:37">
+    <row r="86" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>83</v>
       </c>
@@ -11761,7 +11869,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="87" spans="1:37">
+    <row r="87" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>84</v>
       </c>
@@ -11871,7 +11979,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="88" spans="1:37">
+    <row r="88" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>85</v>
       </c>
@@ -11981,7 +12089,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="89" spans="1:37">
+    <row r="89" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>86</v>
       </c>
@@ -12094,7 +12202,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="90" spans="1:37">
+    <row r="90" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>87</v>
       </c>
@@ -12204,7 +12312,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="91" spans="1:37">
+    <row r="91" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>88</v>
       </c>
@@ -12317,7 +12425,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="92" spans="1:37">
+    <row r="92" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>89</v>
       </c>
@@ -12427,7 +12535,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="93" spans="1:37">
+    <row r="93" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>90</v>
       </c>
@@ -12537,7 +12645,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="94" spans="1:37">
+    <row r="94" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>92</v>
       </c>
@@ -12644,7 +12752,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="95" spans="1:37">
+    <row r="95" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
@@ -12751,7 +12859,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="96" spans="1:37">
+    <row r="96" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
@@ -12858,7 +12966,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:36">
+    <row r="97" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
@@ -12965,7 +13073,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="98" spans="1:36">
+    <row r="98" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
@@ -13072,7 +13180,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="99" spans="1:36">
+    <row r="99" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
@@ -13179,7 +13287,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="100" spans="1:36">
+    <row r="100" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>98</v>
       </c>
@@ -13286,7 +13394,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="101" spans="1:36">
+    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
@@ -13393,7 +13501,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="102" spans="1:36">
+    <row r="102" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A102">
         <v>100</v>
       </c>
@@ -13500,7 +13608,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="103" spans="1:36">
+    <row r="103" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A103">
         <v>101</v>
       </c>
@@ -13607,7 +13715,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="104" spans="1:36">
+    <row r="104" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A104">
         <v>102</v>
       </c>
@@ -13714,7 +13822,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="105" spans="1:36">
+    <row r="105" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A105">
         <v>103</v>
       </c>
@@ -13821,7 +13929,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="106" spans="1:36">
+    <row r="106" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A106">
         <v>104</v>
       </c>
@@ -13928,7 +14036,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="107" spans="1:36">
+    <row r="107" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A107">
         <v>105</v>
       </c>
@@ -14035,7 +14143,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="108" spans="1:36">
+    <row r="108" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A108">
         <v>106</v>
       </c>
@@ -14142,7 +14250,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="109" spans="1:36">
+    <row r="109" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A109">
         <v>107</v>
       </c>
@@ -14249,7 +14357,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="110" spans="1:36">
+    <row r="110" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A110">
         <v>108</v>
       </c>
@@ -14356,7 +14464,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:36">
+    <row r="111" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A111">
         <v>109</v>
       </c>
@@ -14463,7 +14571,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="112" spans="1:36">
+    <row r="112" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A112">
         <v>110</v>
       </c>
@@ -14570,7 +14678,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="113" spans="1:36">
+    <row r="113" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A113">
         <v>111</v>
       </c>
@@ -14677,7 +14785,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:36">
+    <row r="114" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A114">
         <v>112</v>
       </c>
@@ -14784,7 +14892,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="115" spans="1:36">
+    <row r="115" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A115">
         <v>113</v>
       </c>
@@ -14891,7 +14999,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="116" spans="1:36">
+    <row r="116" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A116">
         <v>100</v>
       </c>
@@ -15001,7 +15109,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:36">
+    <row r="117" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A117">
         <v>114</v>
       </c>
@@ -15111,7 +15219,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="118" spans="1:36">
+    <row r="118" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A118">
         <v>115</v>
       </c>
@@ -15221,7 +15329,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="119" spans="1:36">
+    <row r="119" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A119">
         <v>116</v>
       </c>
@@ -15331,7 +15439,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="120" spans="1:36">
+    <row r="120" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A120">
         <v>117</v>
       </c>
@@ -15441,7 +15549,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="121" spans="1:36">
+    <row r="121" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A121">
         <v>118</v>
       </c>
@@ -15551,7 +15659,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="122" spans="1:36">
+    <row r="122" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A122">
         <v>119</v>
       </c>
@@ -15661,7 +15769,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="123" spans="1:36">
+    <row r="123" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A123">
         <v>120</v>
       </c>
@@ -15771,7 +15879,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="124" spans="1:36">
+    <row r="124" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A124">
         <v>121</v>
       </c>
@@ -15881,7 +15989,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="125" spans="1:36">
+    <row r="125" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A125">
         <v>122</v>
       </c>
@@ -15991,7 +16099,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="126" spans="1:36">
+    <row r="126" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A126">
         <v>123</v>
       </c>
@@ -16101,7 +16209,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="127" spans="1:36">
+    <row r="127" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A127">
         <v>124</v>
       </c>
@@ -16211,7 +16319,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="128" spans="1:36">
+    <row r="128" spans="1:36" x14ac:dyDescent="0.2">
       <c r="A128">
         <v>125</v>
       </c>
@@ -16321,7 +16429,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="129" spans="1:37">
+    <row r="129" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A129">
         <v>126</v>
       </c>
@@ -16431,7 +16539,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="130" spans="1:37">
+    <row r="130" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A130">
         <v>127</v>
       </c>
@@ -16541,7 +16649,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="131" spans="1:37">
+    <row r="131" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A131">
         <v>128</v>
       </c>
@@ -16651,7 +16759,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="132" spans="1:37">
+    <row r="132" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A132">
         <v>129</v>
       </c>
@@ -16761,7 +16869,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="133" spans="1:37">
+    <row r="133" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A133">
         <v>130</v>
       </c>
@@ -16871,7 +16979,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="134" spans="1:37">
+    <row r="134" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A134">
         <v>131</v>
       </c>
@@ -16981,7 +17089,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="135" spans="1:37">
+    <row r="135" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A135">
         <v>132</v>
       </c>
@@ -17091,7 +17199,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="136" spans="1:37">
+    <row r="136" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A136">
         <v>133</v>
       </c>
@@ -17201,7 +17309,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="137" spans="1:37">
+    <row r="137" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A137">
         <v>134</v>
       </c>
@@ -17311,7 +17419,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="138" spans="1:37">
+    <row r="138" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A138">
         <v>135</v>
       </c>
@@ -17421,7 +17529,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="139" spans="1:37">
+    <row r="139" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A139">
         <v>136</v>
       </c>
@@ -17531,7 +17639,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="140" spans="1:37">
+    <row r="140" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A140">
         <v>137</v>
       </c>
@@ -17641,7 +17749,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="141" spans="1:37">
+    <row r="141" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A141">
         <v>138</v>
       </c>
@@ -17751,7 +17859,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="142" spans="1:37">
+    <row r="142" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A142">
         <v>139</v>
       </c>
@@ -17861,7 +17969,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="143" spans="1:37">
+    <row r="143" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A143">
         <v>140</v>
       </c>
@@ -17971,7 +18079,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="144" spans="1:37">
+    <row r="144" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A144">
         <v>141</v>
       </c>
@@ -18081,7 +18189,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="145" spans="1:37">
+    <row r="145" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A145">
         <v>142</v>
       </c>
@@ -18191,7 +18299,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="146" spans="1:37">
+    <row r="146" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A146">
         <v>143</v>
       </c>
@@ -18301,7 +18409,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="147" spans="1:37">
+    <row r="147" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A147">
         <v>144</v>
       </c>
@@ -18411,7 +18519,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="148" spans="1:37">
+    <row r="148" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A148">
         <v>145</v>
       </c>
@@ -18521,7 +18629,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="149" spans="1:37">
+    <row r="149" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A149">
         <v>146</v>
       </c>
@@ -18631,7 +18739,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="150" spans="1:37">
+    <row r="150" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A150">
         <v>147</v>
       </c>
@@ -18738,7 +18846,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="151" spans="1:37">
+    <row r="151" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A151">
         <v>148</v>
       </c>
@@ -18845,7 +18953,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="152" spans="1:37">
+    <row r="152" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A152">
         <v>149</v>
       </c>
@@ -18952,7 +19060,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="153" spans="1:37">
+    <row r="153" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A153">
         <v>150</v>
       </c>
@@ -19059,7 +19167,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="154" spans="1:37">
+    <row r="154" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A154">
         <v>151</v>
       </c>
@@ -19103,7 +19211,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="155" spans="1:37">
+    <row r="155" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A155">
         <v>152</v>
       </c>
@@ -19147,7 +19255,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="156" spans="1:37">
+    <row r="156" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A156">
         <v>153</v>
       </c>
@@ -19191,7 +19299,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="157" spans="1:37">
+    <row r="157" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A157">
         <v>154</v>
       </c>
@@ -19235,7 +19343,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="158" spans="1:37">
+    <row r="158" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A158">
         <v>155</v>
       </c>
@@ -19279,7 +19387,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="159" spans="1:37">
+    <row r="159" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A159">
         <v>156</v>
       </c>
@@ -19323,7 +19431,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="160" spans="1:37">
+    <row r="160" spans="1:37" x14ac:dyDescent="0.2">
       <c r="A160">
         <v>157</v>
       </c>
@@ -19367,7 +19475,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="161" spans="1:14">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A161">
         <v>158</v>
       </c>
@@ -19411,7 +19519,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="162" spans="1:14">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A162">
         <v>159</v>
       </c>
@@ -19455,7 +19563,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="163" spans="1:14">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A163">
         <v>160</v>
       </c>
@@ -19499,7 +19607,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="164" spans="1:14">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A164">
         <v>161</v>
       </c>
@@ -19543,7 +19651,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="165" spans="1:14">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A165">
         <v>162</v>
       </c>
@@ -19585,6 +19693,294 @@
       </c>
       <c r="N165" t="s">
         <v>40</v>
+      </c>
+    </row>
+    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A166">
+        <v>163</v>
+      </c>
+      <c r="B166" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A167">
+        <v>164</v>
+      </c>
+      <c r="B167" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A168">
+        <v>165</v>
+      </c>
+      <c r="B168" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A169">
+        <v>166</v>
+      </c>
+      <c r="B169" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A170">
+        <v>167</v>
+      </c>
+      <c r="B170" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A171">
+        <v>168</v>
+      </c>
+      <c r="B171" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A172">
+        <v>169</v>
+      </c>
+      <c r="B172" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A173">
+        <v>170</v>
+      </c>
+      <c r="B173" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A174">
+        <v>171</v>
+      </c>
+      <c r="B174" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A175">
+        <v>172</v>
+      </c>
+      <c r="B175" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="A176">
+        <v>173</v>
+      </c>
+      <c r="B176" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A177">
+        <v>174</v>
+      </c>
+      <c r="B177" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A178">
+        <v>175</v>
+      </c>
+      <c r="B178" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A179">
+        <v>176</v>
+      </c>
+      <c r="B179" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A180">
+        <v>177</v>
+      </c>
+      <c r="B180" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A181">
+        <v>178</v>
+      </c>
+      <c r="B181" t="s">
+        <v>489</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A182">
+        <v>179</v>
+      </c>
+      <c r="B182" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A183">
+        <v>180</v>
+      </c>
+      <c r="B183" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A184">
+        <v>181</v>
+      </c>
+      <c r="B184" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A185">
+        <v>182</v>
+      </c>
+      <c r="B185" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A186">
+        <v>183</v>
+      </c>
+      <c r="B186" t="s">
+        <v>494</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A187">
+        <v>184</v>
+      </c>
+      <c r="B187" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A188">
+        <v>185</v>
+      </c>
+      <c r="B188" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A189">
+        <v>186</v>
+      </c>
+      <c r="B189" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A190">
+        <v>187</v>
+      </c>
+      <c r="B190" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A191">
+        <v>188</v>
+      </c>
+      <c r="B191" t="s">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A192">
+        <v>189</v>
+      </c>
+      <c r="B192" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A193">
+        <v>190</v>
+      </c>
+      <c r="B193" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A194">
+        <v>191</v>
+      </c>
+      <c r="B194" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A195">
+        <v>192</v>
+      </c>
+      <c r="B195" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A196">
+        <v>193</v>
+      </c>
+      <c r="B196" t="s">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A197">
+        <v>194</v>
+      </c>
+      <c r="B197" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A198">
+        <v>195</v>
+      </c>
+      <c r="B198" t="s">
+        <v>506</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A199">
+        <v>196</v>
+      </c>
+      <c r="B199" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A200">
+        <v>197</v>
+      </c>
+      <c r="B200" t="s">
+        <v>508</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A201">
+        <v>198</v>
+      </c>
+      <c r="B201" t="s">
+        <v>509</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add inventory (y/n if have, etc.) that Jon helped with, so far
</commit_message>
<xml_diff>
--- a/botanical-collections_rvm.xlsx
+++ b/botanical-collections_rvm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\botanical-collections\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7C9B38-7D37-49E4-A82D-7B3522E48FFB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F94B76CD-B97D-48C3-A9B7-97C072795A40}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4810" uniqueCount="523">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4866" uniqueCount="523">
   <si>
     <t>collection_no</t>
   </si>
@@ -2474,10 +2474,10 @@
   <dimension ref="A1:AL204"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="AJ3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="J87" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AL69" sqref="AL69"/>
+      <selection pane="bottomRight" activeCell="AD48" sqref="AD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2789,6 +2789,9 @@
       <c r="AJ3" s="9">
         <v>3</v>
       </c>
+      <c r="AL3" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="4" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9">
@@ -2902,6 +2905,9 @@
       <c r="AK4" s="9" t="s">
         <v>69</v>
       </c>
+      <c r="AL4" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="5" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="9">
@@ -3125,6 +3131,9 @@
       <c r="AJ6" s="9" t="s">
         <v>88</v>
       </c>
+      <c r="AL6" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="7" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9">
@@ -3235,6 +3244,9 @@
       <c r="AJ7" s="9" t="s">
         <v>88</v>
       </c>
+      <c r="AL7" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="8" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9">
@@ -3345,6 +3357,9 @@
       <c r="AJ8" s="9" t="s">
         <v>88</v>
       </c>
+      <c r="AL8" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="9" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9">
@@ -3452,6 +3467,9 @@
       <c r="AJ9" s="9" t="s">
         <v>88</v>
       </c>
+      <c r="AL9" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="10" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="9">
@@ -3556,6 +3574,9 @@
       <c r="AJ10" s="9" t="s">
         <v>113</v>
       </c>
+      <c r="AL10" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="11" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
@@ -3660,6 +3681,9 @@
       <c r="AJ11" s="9" t="s">
         <v>113</v>
       </c>
+      <c r="AL11" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="12" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A12" s="9">
@@ -3770,6 +3794,9 @@
       <c r="AJ12" s="9" t="s">
         <v>88</v>
       </c>
+      <c r="AL12" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="13" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9">
@@ -3880,6 +3907,9 @@
       <c r="AJ13" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL13" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="14" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="9">
@@ -3984,6 +4014,9 @@
       <c r="AJ14" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL14" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="15" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
@@ -4088,6 +4121,9 @@
       <c r="AJ15" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL15" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="16" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9">
@@ -4192,6 +4228,9 @@
       <c r="AJ16" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL16" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="17" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9">
@@ -4412,6 +4451,9 @@
       <c r="AJ18" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL18" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="19" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A19" s="9">
@@ -4522,6 +4564,9 @@
       <c r="AJ19" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL19" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="20" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A20" s="9">
@@ -4632,6 +4677,9 @@
       <c r="AJ20" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL20" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="21" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A21" s="9">
@@ -4855,6 +4903,9 @@
       <c r="AJ22" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL22" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="23" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="9">
@@ -4965,6 +5016,9 @@
       <c r="AJ23" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL23" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="24" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A24" s="9">
@@ -5188,6 +5242,9 @@
       <c r="AJ25" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL25" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="26" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="9">
@@ -5518,6 +5575,9 @@
       <c r="AJ28" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL28" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="29" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="9">
@@ -5628,6 +5688,9 @@
       <c r="AJ29" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL29" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="30" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A30" s="9">
@@ -5851,6 +5914,9 @@
       <c r="AK31" s="9" t="s">
         <v>200</v>
       </c>
+      <c r="AL31" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="32" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A32" s="9">
@@ -5964,6 +6030,9 @@
       <c r="AK32" s="9" t="s">
         <v>200</v>
       </c>
+      <c r="AL32" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="33" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A33" s="9">
@@ -6077,6 +6146,9 @@
       <c r="AK33" s="9" t="s">
         <v>200</v>
       </c>
+      <c r="AL33" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="34" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A34" s="9">
@@ -6300,6 +6372,9 @@
       <c r="AJ35" s="9">
         <v>3</v>
       </c>
+      <c r="AL35" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="36" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A36" s="9">
@@ -6410,6 +6485,9 @@
       <c r="AJ36" s="9">
         <v>3</v>
       </c>
+      <c r="AL36" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="37" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A37" s="9">
@@ -6520,6 +6598,9 @@
       <c r="AJ37" s="9">
         <v>3</v>
       </c>
+      <c r="AL37" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="38" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A38" s="9">
@@ -7076,6 +7157,9 @@
       <c r="AJ42" s="9">
         <v>3</v>
       </c>
+      <c r="AL42" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="43" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9">
@@ -7519,6 +7603,9 @@
       <c r="AJ46" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL46" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="47" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A47" s="9">
@@ -7629,6 +7716,9 @@
       <c r="AJ47" s="9" t="s">
         <v>250</v>
       </c>
+      <c r="AL47" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="48" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9">
@@ -7739,8 +7829,11 @@
       <c r="AJ48" s="9" t="s">
         <v>250</v>
       </c>
+      <c r="AL48" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="49" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A49" s="9">
         <v>41</v>
       </c>
@@ -7849,8 +7942,11 @@
       <c r="AJ49" s="9" t="s">
         <v>256</v>
       </c>
+      <c r="AL49" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="50" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A50" s="9">
         <v>42</v>
       </c>
@@ -7959,8 +8055,11 @@
       <c r="AJ50" s="9" t="s">
         <v>256</v>
       </c>
+      <c r="AL50" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="51" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A51" s="9">
         <v>43</v>
       </c>
@@ -8069,8 +8168,11 @@
       <c r="AJ51" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL51" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="52" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A52" s="9">
         <v>44</v>
       </c>
@@ -8180,7 +8282,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A53" s="9">
         <v>45</v>
       </c>
@@ -8290,7 +8392,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A54" s="9">
         <v>46</v>
       </c>
@@ -8399,8 +8501,11 @@
       <c r="AJ54" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL54" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="55" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A55" s="9">
         <v>47</v>
       </c>
@@ -8509,8 +8614,11 @@
       <c r="AJ55" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL55" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="56" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9">
         <v>48</v>
       </c>
@@ -8622,8 +8730,11 @@
       <c r="AK56" s="9" t="s">
         <v>200</v>
       </c>
+      <c r="AL56" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="57" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A57" s="9">
         <v>49</v>
       </c>
@@ -8735,8 +8846,11 @@
       <c r="AK57" s="9" t="s">
         <v>200</v>
       </c>
+      <c r="AL57" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="58" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A58" s="9">
         <v>50</v>
       </c>
@@ -8848,8 +8962,11 @@
       <c r="AK58" s="9" t="s">
         <v>200</v>
       </c>
+      <c r="AL58" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="59" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A59" s="9">
         <v>51</v>
       </c>
@@ -8961,8 +9078,11 @@
       <c r="AK59" s="9" t="s">
         <v>200</v>
       </c>
+      <c r="AL59" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="60" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9">
         <v>54</v>
       </c>
@@ -9072,7 +9192,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A61" s="9">
         <v>55</v>
       </c>
@@ -9182,7 +9302,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A62" s="9">
         <v>56</v>
       </c>
@@ -9291,8 +9411,11 @@
       <c r="AJ62" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL62" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="63" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A63" s="9">
         <v>57</v>
       </c>
@@ -9401,8 +9524,11 @@
       <c r="AJ63" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL63" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
-    <row r="64" spans="1:37" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A64" s="9">
         <v>58</v>
       </c>
@@ -10070,6 +10196,9 @@
       <c r="AJ69" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL69" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="70" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A70" s="9">
@@ -10180,6 +10309,9 @@
       <c r="AJ70" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL70" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="71" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A71" s="9">
@@ -10290,6 +10422,9 @@
       <c r="AJ71" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL71" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="72" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A72" s="9">
@@ -10400,6 +10535,9 @@
       <c r="AJ72" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL72" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="73" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9">
@@ -10507,6 +10645,9 @@
       <c r="AJ73" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL73" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="74" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A74" s="9">
@@ -10614,6 +10755,9 @@
       <c r="AJ74" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL74" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="75" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A75" s="9">
@@ -10721,6 +10865,9 @@
       <c r="AJ75" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL75" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="76" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A76" s="9">
@@ -10938,6 +11085,9 @@
       <c r="AJ77" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL77" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="78" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A78" s="9">
@@ -11048,6 +11198,9 @@
       <c r="AJ78" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL78" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="79" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A79" s="9">
@@ -11378,6 +11531,9 @@
       <c r="AJ81" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL81" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="82" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A82" s="9">
@@ -11708,6 +11864,9 @@
       <c r="AJ84" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL84" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="85" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A85" s="9">
@@ -12484,6 +12643,9 @@
       <c r="AJ91" s="9" t="s">
         <v>81</v>
       </c>
+      <c r="AL91" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="92" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A92" s="9">
@@ -12820,6 +12982,9 @@
       <c r="AK94" s="9" t="s">
         <v>200</v>
       </c>
+      <c r="AL94" s="9" t="s">
+        <v>522</v>
+      </c>
     </row>
     <row r="95" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A95" s="9">
@@ -12929,6 +13094,9 @@
       </c>
       <c r="AJ95" s="9" t="s">
         <v>81</v>
+      </c>
+      <c r="AL95" s="9" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="96" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Open and close .xlsx-file
</commit_message>
<xml_diff>
--- a/botanical-collections_rvm.xlsx
+++ b/botanical-collections_rvm.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Desktop\botanical-collections\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruanvanmazijk/botanical-collections/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674E2E06-BA72-4443-9810-D4D4815E6BCA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FFF8AA-293B-4949-BA20-CB4506CD4377}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1660" yWindow="-20020" windowWidth="25600" windowHeight="20020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="botanical-collections_rvm" sheetId="1" r:id="rId1"/>
@@ -1598,7 +1598,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -2477,54 +2477,54 @@
   <dimension ref="A1:AL204"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="J24" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B183" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="L36" sqref="L36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="45.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="37.88671875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="68.6640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="37.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5703125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="11" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="12.109375" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="6.140625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.28515625" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="29" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="52.33203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="52.28515625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="157" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="42.33203125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="144.44140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="167.88671875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="42.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="144.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="167.85546875" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="49" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="46.5546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="46.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38">
       <c r="B1" s="6" t="s">
         <v>468</v>
       </c>
@@ -2567,7 +2567,7 @@
       <c r="AI1" s="2"/>
       <c r="AJ1" s="3"/>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2683,7 +2683,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="3" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" s="9" customFormat="1">
       <c r="A3" s="9">
         <v>1</v>
       </c>
@@ -2796,7 +2796,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="4" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" s="9" customFormat="1">
       <c r="A4" s="9">
         <v>2</v>
       </c>
@@ -2912,7 +2912,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="5" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" s="9" customFormat="1">
       <c r="A5" s="9">
         <v>3</v>
       </c>
@@ -3025,7 +3025,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="6" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" s="9" customFormat="1">
       <c r="A6" s="9">
         <v>4</v>
       </c>
@@ -3138,7 +3138,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="7" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38" s="9" customFormat="1">
       <c r="A7" s="9">
         <v>5</v>
       </c>
@@ -3251,7 +3251,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="8" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38" s="9" customFormat="1">
       <c r="A8" s="9">
         <v>6</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="9" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:38" s="9" customFormat="1">
       <c r="A9" s="9">
         <v>7</v>
       </c>
@@ -3474,7 +3474,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="10" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:38" s="9" customFormat="1">
       <c r="A10" s="9">
         <v>8</v>
       </c>
@@ -3581,7 +3581,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="11" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:38" s="9" customFormat="1">
       <c r="A11" s="9" t="s">
         <v>519</v>
       </c>
@@ -3688,7 +3688,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="12" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38" s="9" customFormat="1">
       <c r="A12" s="9">
         <v>9</v>
       </c>
@@ -3801,7 +3801,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="13" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" s="9" customFormat="1">
       <c r="A13" s="9">
         <v>10</v>
       </c>
@@ -3914,7 +3914,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="14" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38" s="9" customFormat="1">
       <c r="A14" s="9">
         <v>11</v>
       </c>
@@ -4021,7 +4021,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="15" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" s="9" customFormat="1">
       <c r="A15" s="9" t="s">
         <v>517</v>
       </c>
@@ -4128,7 +4128,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="16" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" s="9" customFormat="1">
       <c r="A16" s="9">
         <v>12</v>
       </c>
@@ -4235,7 +4235,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="17" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" s="9" customFormat="1">
       <c r="A17" s="9">
         <v>13</v>
       </c>
@@ -4345,7 +4345,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:38" s="9" customFormat="1">
       <c r="A18" s="9">
         <v>14</v>
       </c>
@@ -4458,7 +4458,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="19" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38" s="9" customFormat="1">
       <c r="A19" s="9">
         <v>15</v>
       </c>
@@ -4571,7 +4571,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="20" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38" s="9" customFormat="1">
       <c r="A20" s="9">
         <v>16</v>
       </c>
@@ -4684,7 +4684,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="21" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:38" s="9" customFormat="1">
       <c r="A21" s="9">
         <v>17</v>
       </c>
@@ -4797,7 +4797,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="22" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:38" s="9" customFormat="1">
       <c r="A22" s="9">
         <v>18</v>
       </c>
@@ -4910,7 +4910,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="23" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" s="9" customFormat="1">
       <c r="A23" s="9">
         <v>19</v>
       </c>
@@ -5023,7 +5023,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="24" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38" s="9" customFormat="1">
       <c r="A24" s="9">
         <v>20</v>
       </c>
@@ -5136,7 +5136,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="25" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38" s="9" customFormat="1">
       <c r="A25" s="9">
         <v>21</v>
       </c>
@@ -5249,7 +5249,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="26" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38" s="9" customFormat="1">
       <c r="A26" s="9">
         <v>22</v>
       </c>
@@ -5359,7 +5359,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" s="9" customFormat="1">
       <c r="A27" s="9">
         <v>23</v>
       </c>
@@ -5469,7 +5469,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="28" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:38" s="9" customFormat="1">
       <c r="A28" s="9">
         <v>24</v>
       </c>
@@ -5582,7 +5582,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="29" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:38" s="9" customFormat="1">
       <c r="A29" s="9">
         <v>25</v>
       </c>
@@ -5695,7 +5695,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="30" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:38" s="9" customFormat="1">
       <c r="A30" s="9">
         <v>26</v>
       </c>
@@ -5805,7 +5805,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="31" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38" s="9" customFormat="1">
       <c r="A31" s="9">
         <v>27</v>
       </c>
@@ -5921,7 +5921,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="32" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:38" s="9" customFormat="1">
       <c r="A32" s="9">
         <v>28</v>
       </c>
@@ -6037,7 +6037,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="33" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38" s="9" customFormat="1">
       <c r="A33" s="9">
         <v>29</v>
       </c>
@@ -6153,7 +6153,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="34" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:38" s="9" customFormat="1">
       <c r="A34" s="9">
         <v>30</v>
       </c>
@@ -6266,7 +6266,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="35" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:38" s="9" customFormat="1">
       <c r="A35" s="9">
         <v>31</v>
       </c>
@@ -6379,7 +6379,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="36" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:38" s="9" customFormat="1">
       <c r="A36" s="9">
         <v>32</v>
       </c>
@@ -6492,7 +6492,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="37" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38" s="9" customFormat="1">
       <c r="A37" s="9">
         <v>33</v>
       </c>
@@ -6605,7 +6605,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="38" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" s="9" customFormat="1">
       <c r="A38" s="9">
         <v>34</v>
       </c>
@@ -6721,7 +6721,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="39" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" s="9" customFormat="1">
       <c r="A39" s="9">
         <v>35</v>
       </c>
@@ -6831,7 +6831,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="40" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:38" s="9" customFormat="1">
       <c r="A40" s="9">
         <v>36</v>
       </c>
@@ -6941,7 +6941,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="41" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:38" s="9" customFormat="1">
       <c r="A41" s="9">
         <v>37</v>
       </c>
@@ -7051,7 +7051,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="42" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" s="9" customFormat="1">
       <c r="A42" s="9">
         <v>38</v>
       </c>
@@ -7164,7 +7164,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="43" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:38" s="9" customFormat="1">
       <c r="A43" s="9">
         <v>39</v>
       </c>
@@ -7277,7 +7277,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="44" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:38" s="9" customFormat="1">
       <c r="A44" s="9">
         <v>40</v>
       </c>
@@ -7387,7 +7387,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" s="9" customFormat="1">
       <c r="A45" s="9" t="s">
         <v>507</v>
       </c>
@@ -7497,7 +7497,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="46" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:38" s="9" customFormat="1">
       <c r="A46" s="9" t="s">
         <v>510</v>
       </c>
@@ -7610,7 +7610,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="47" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" s="9" customFormat="1">
       <c r="A47" s="9">
         <v>53</v>
       </c>
@@ -7723,7 +7723,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="48" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:38" s="9" customFormat="1">
       <c r="A48" s="9">
         <v>91</v>
       </c>
@@ -7836,7 +7836,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="49" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:38" s="9" customFormat="1">
       <c r="A49" s="9">
         <v>41</v>
       </c>
@@ -7949,7 +7949,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="50" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:38" s="9" customFormat="1">
       <c r="A50" s="9">
         <v>42</v>
       </c>
@@ -8062,7 +8062,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="51" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:38" s="9" customFormat="1">
       <c r="A51" s="9">
         <v>43</v>
       </c>
@@ -8175,7 +8175,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="52" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:38" s="9" customFormat="1">
       <c r="A52" s="9">
         <v>44</v>
       </c>
@@ -8285,7 +8285,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="53" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:38" s="9" customFormat="1">
       <c r="A53" s="9">
         <v>45</v>
       </c>
@@ -8395,7 +8395,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:38" s="9" customFormat="1">
       <c r="A54" s="9">
         <v>46</v>
       </c>
@@ -8508,7 +8508,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="55" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:38" s="9" customFormat="1">
       <c r="A55" s="9">
         <v>47</v>
       </c>
@@ -8621,7 +8621,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="56" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:38" s="9" customFormat="1">
       <c r="A56" s="9">
         <v>48</v>
       </c>
@@ -8737,7 +8737,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="57" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:38" s="9" customFormat="1">
       <c r="A57" s="9">
         <v>49</v>
       </c>
@@ -8853,7 +8853,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="58" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:38" s="9" customFormat="1">
       <c r="A58" s="9">
         <v>50</v>
       </c>
@@ -8969,7 +8969,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="59" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:38" s="9" customFormat="1">
       <c r="A59" s="9">
         <v>51</v>
       </c>
@@ -9085,7 +9085,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="60" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:38" s="9" customFormat="1">
       <c r="A60" s="9">
         <v>54</v>
       </c>
@@ -9195,7 +9195,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="61" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:38" s="9" customFormat="1">
       <c r="A61" s="9">
         <v>55</v>
       </c>
@@ -9305,7 +9305,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="62" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:38" s="9" customFormat="1">
       <c r="A62" s="9">
         <v>56</v>
       </c>
@@ -9418,7 +9418,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="63" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:38" s="9" customFormat="1">
       <c r="A63" s="9">
         <v>57</v>
       </c>
@@ -9531,7 +9531,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="64" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:38" s="9" customFormat="1">
       <c r="A64" s="9">
         <v>58</v>
       </c>
@@ -9641,7 +9641,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="65" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:38" s="9" customFormat="1">
       <c r="A65" s="9">
         <v>59</v>
       </c>
@@ -9751,7 +9751,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="66" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:38" s="9" customFormat="1">
       <c r="A66" s="9">
         <v>60</v>
       </c>
@@ -9864,7 +9864,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="67" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:38" s="9" customFormat="1">
       <c r="A67" s="9">
         <v>61</v>
       </c>
@@ -9977,7 +9977,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="68" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:38" s="9" customFormat="1">
       <c r="A68" s="9">
         <v>62</v>
       </c>
@@ -10090,7 +10090,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="69" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:38" s="9" customFormat="1">
       <c r="A69" s="9">
         <v>63</v>
       </c>
@@ -10203,7 +10203,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="70" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:38" s="9" customFormat="1">
       <c r="A70" s="9">
         <v>64</v>
       </c>
@@ -10316,7 +10316,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="71" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:38" s="9" customFormat="1">
       <c r="A71" s="9">
         <v>65</v>
       </c>
@@ -10429,7 +10429,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="72" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:38" s="9" customFormat="1">
       <c r="A72" s="9">
         <v>66</v>
       </c>
@@ -10542,7 +10542,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="73" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:38" s="9" customFormat="1">
       <c r="A73" s="9">
         <v>67</v>
       </c>
@@ -10652,7 +10652,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="74" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:38" s="9" customFormat="1">
       <c r="A74" s="9">
         <v>68</v>
       </c>
@@ -10762,7 +10762,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="75" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:38" s="9" customFormat="1">
       <c r="A75" s="9">
         <v>69</v>
       </c>
@@ -10872,7 +10872,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="76" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:38" s="9" customFormat="1">
       <c r="A76" s="9">
         <v>70</v>
       </c>
@@ -10979,7 +10979,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="77" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:38" s="9" customFormat="1">
       <c r="A77" s="9">
         <v>71</v>
       </c>
@@ -11092,7 +11092,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="78" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:38" s="9" customFormat="1">
       <c r="A78" s="9">
         <v>72</v>
       </c>
@@ -11205,7 +11205,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="79" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:38" s="9" customFormat="1">
       <c r="A79" s="9">
         <v>73</v>
       </c>
@@ -11315,7 +11315,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="80" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:38" s="9" customFormat="1">
       <c r="A80" s="9">
         <v>74</v>
       </c>
@@ -11425,7 +11425,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="81" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:38" s="9" customFormat="1">
       <c r="A81" s="9">
         <v>75</v>
       </c>
@@ -11538,7 +11538,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="82" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:38" s="9" customFormat="1">
       <c r="A82" s="9">
         <v>76</v>
       </c>
@@ -11648,7 +11648,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="83" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:38" s="9" customFormat="1">
       <c r="A83" s="9">
         <v>77</v>
       </c>
@@ -11758,7 +11758,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="84" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:38" s="9" customFormat="1">
       <c r="A84" s="9">
         <v>78</v>
       </c>
@@ -11871,7 +11871,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="85" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:38" s="9" customFormat="1">
       <c r="A85" s="9">
         <v>79</v>
       </c>
@@ -11981,7 +11981,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="86" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:38" s="9" customFormat="1">
       <c r="A86" s="9">
         <v>80</v>
       </c>
@@ -12091,7 +12091,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:38" s="9" customFormat="1">
       <c r="A87" s="9">
         <v>81</v>
       </c>
@@ -12201,7 +12201,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="88" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:38" s="9" customFormat="1">
       <c r="A88" s="9">
         <v>82</v>
       </c>
@@ -12314,7 +12314,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="89" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:38" s="9" customFormat="1">
       <c r="A89" s="9">
         <v>83</v>
       </c>
@@ -12427,7 +12427,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="90" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:38" s="9" customFormat="1">
       <c r="A90" s="9">
         <v>84</v>
       </c>
@@ -12537,7 +12537,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="91" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:38" s="9" customFormat="1">
       <c r="A91" s="9">
         <v>85</v>
       </c>
@@ -12650,7 +12650,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="92" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:38" s="9" customFormat="1">
       <c r="A92" s="9">
         <v>86</v>
       </c>
@@ -12763,7 +12763,7 @@
         <v>343</v>
       </c>
     </row>
-    <row r="93" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:38" s="9" customFormat="1">
       <c r="A93" s="9">
         <v>87</v>
       </c>
@@ -12873,7 +12873,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="94" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:38" s="9" customFormat="1">
       <c r="A94" s="9">
         <v>88</v>
       </c>
@@ -12989,7 +12989,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="95" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:38" s="9" customFormat="1">
       <c r="A95" s="9">
         <v>89</v>
       </c>
@@ -13102,7 +13102,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="96" spans="1:38" s="9" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:38" s="9" customFormat="1">
       <c r="A96" s="9">
         <v>90</v>
       </c>
@@ -13212,7 +13212,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="97" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:36">
       <c r="A97">
         <v>92</v>
       </c>
@@ -13319,7 +13319,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="98" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:36">
       <c r="A98">
         <v>93</v>
       </c>
@@ -13426,7 +13426,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="99" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:36">
       <c r="A99">
         <v>94</v>
       </c>
@@ -13533,7 +13533,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="100" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:36">
       <c r="A100">
         <v>95</v>
       </c>
@@ -13640,7 +13640,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="101" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:36">
       <c r="A101">
         <v>96</v>
       </c>
@@ -13747,7 +13747,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="102" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:36">
       <c r="A102">
         <v>97</v>
       </c>
@@ -13854,7 +13854,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="103" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:36">
       <c r="A103">
         <v>98</v>
       </c>
@@ -13961,7 +13961,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="104" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:36">
       <c r="A104">
         <v>99</v>
       </c>
@@ -14068,7 +14068,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="105" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:36">
       <c r="A105">
         <v>100</v>
       </c>
@@ -14175,7 +14175,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="106" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:36">
       <c r="A106">
         <v>101</v>
       </c>
@@ -14282,7 +14282,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="107" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:36">
       <c r="A107">
         <v>102</v>
       </c>
@@ -14389,7 +14389,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="108" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:36">
       <c r="A108">
         <v>103</v>
       </c>
@@ -14496,7 +14496,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="109" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:36">
       <c r="A109">
         <v>104</v>
       </c>
@@ -14603,7 +14603,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="110" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:36">
       <c r="A110">
         <v>105</v>
       </c>
@@ -14710,7 +14710,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="111" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:36">
       <c r="A111">
         <v>106</v>
       </c>
@@ -14817,7 +14817,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="112" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:36">
       <c r="A112">
         <v>107</v>
       </c>
@@ -14924,7 +14924,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="113" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:36">
       <c r="A113">
         <v>108</v>
       </c>
@@ -15031,7 +15031,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="114" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:36">
       <c r="A114">
         <v>109</v>
       </c>
@@ -15138,7 +15138,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="115" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:36">
       <c r="A115">
         <v>110</v>
       </c>
@@ -15245,7 +15245,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="116" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:36">
       <c r="A116">
         <v>111</v>
       </c>
@@ -15352,7 +15352,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="117" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:36">
       <c r="A117">
         <v>112</v>
       </c>
@@ -15459,7 +15459,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="118" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:36">
       <c r="A118">
         <v>113</v>
       </c>
@@ -15566,7 +15566,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="119" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:36">
       <c r="A119">
         <v>100</v>
       </c>
@@ -15676,7 +15676,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="120" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:36">
       <c r="A120">
         <v>114</v>
       </c>
@@ -15786,7 +15786,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="121" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:36">
       <c r="A121">
         <v>115</v>
       </c>
@@ -15896,7 +15896,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="122" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:36">
       <c r="A122">
         <v>116</v>
       </c>
@@ -16006,7 +16006,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="123" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:36">
       <c r="A123">
         <v>117</v>
       </c>
@@ -16116,7 +16116,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="124" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:36">
       <c r="A124">
         <v>118</v>
       </c>
@@ -16226,7 +16226,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="125" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:36">
       <c r="A125">
         <v>119</v>
       </c>
@@ -16336,7 +16336,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="126" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:36">
       <c r="A126">
         <v>120</v>
       </c>
@@ -16446,7 +16446,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="127" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:36">
       <c r="A127">
         <v>121</v>
       </c>
@@ -16556,7 +16556,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="128" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:36">
       <c r="A128">
         <v>122</v>
       </c>
@@ -16666,7 +16666,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="129" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:36">
       <c r="A129">
         <v>123</v>
       </c>
@@ -16776,7 +16776,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="130" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:36">
       <c r="A130">
         <v>124</v>
       </c>
@@ -16886,7 +16886,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="131" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:36">
       <c r="A131">
         <v>125</v>
       </c>
@@ -16996,7 +16996,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="132" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:36">
       <c r="A132">
         <v>126</v>
       </c>
@@ -17106,7 +17106,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="133" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:36">
       <c r="A133">
         <v>127</v>
       </c>
@@ -17216,7 +17216,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="134" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:36">
       <c r="A134">
         <v>128</v>
       </c>
@@ -17326,7 +17326,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="135" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:36">
       <c r="A135">
         <v>129</v>
       </c>
@@ -17436,7 +17436,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="136" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:36">
       <c r="A136">
         <v>130</v>
       </c>
@@ -17546,7 +17546,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="137" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:36">
       <c r="A137">
         <v>131</v>
       </c>
@@ -17656,7 +17656,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="138" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:36">
       <c r="A138">
         <v>132</v>
       </c>
@@ -17766,7 +17766,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="139" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:36">
       <c r="A139">
         <v>133</v>
       </c>
@@ -17876,7 +17876,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="140" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:36">
       <c r="A140">
         <v>134</v>
       </c>
@@ -17986,7 +17986,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="141" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:36">
       <c r="A141">
         <v>135</v>
       </c>
@@ -18096,7 +18096,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="142" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:36">
       <c r="A142">
         <v>136</v>
       </c>
@@ -18206,7 +18206,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="143" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:36">
       <c r="A143">
         <v>137</v>
       </c>
@@ -18316,7 +18316,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="144" spans="1:36" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:36">
       <c r="A144">
         <v>138</v>
       </c>
@@ -18426,7 +18426,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="145" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:37">
       <c r="A145">
         <v>139</v>
       </c>
@@ -18536,7 +18536,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="146" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:37">
       <c r="A146">
         <v>140</v>
       </c>
@@ -18646,7 +18646,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="147" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:37">
       <c r="A147">
         <v>141</v>
       </c>
@@ -18756,7 +18756,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="148" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:37">
       <c r="A148">
         <v>142</v>
       </c>
@@ -18866,7 +18866,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="149" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:37">
       <c r="A149">
         <v>143</v>
       </c>
@@ -18976,7 +18976,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="150" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:37">
       <c r="A150">
         <v>144</v>
       </c>
@@ -19086,7 +19086,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="151" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:37">
       <c r="A151">
         <v>145</v>
       </c>
@@ -19196,7 +19196,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="152" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:37">
       <c r="A152">
         <v>146</v>
       </c>
@@ -19306,7 +19306,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="153" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:37">
       <c r="A153">
         <v>147</v>
       </c>
@@ -19413,7 +19413,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="154" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:37">
       <c r="A154">
         <v>148</v>
       </c>
@@ -19520,7 +19520,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="155" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:37">
       <c r="A155">
         <v>149</v>
       </c>
@@ -19627,7 +19627,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="156" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:37">
       <c r="A156">
         <v>150</v>
       </c>
@@ -19734,7 +19734,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="157" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:37">
       <c r="A157">
         <v>151</v>
       </c>
@@ -19778,7 +19778,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="158" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:37">
       <c r="A158">
         <v>152</v>
       </c>
@@ -19822,7 +19822,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="159" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:37">
       <c r="A159">
         <v>153</v>
       </c>
@@ -19866,7 +19866,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="160" spans="1:37" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:37">
       <c r="A160">
         <v>154</v>
       </c>
@@ -19910,7 +19910,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:14">
       <c r="A161">
         <v>155</v>
       </c>
@@ -19954,7 +19954,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:14">
       <c r="A162">
         <v>156</v>
       </c>
@@ -19998,7 +19998,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:14">
       <c r="A163">
         <v>157</v>
       </c>
@@ -20042,7 +20042,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:14">
       <c r="A164">
         <v>158</v>
       </c>
@@ -20086,7 +20086,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:14">
       <c r="A165">
         <v>159</v>
       </c>
@@ -20130,7 +20130,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:14">
       <c r="A166">
         <v>160</v>
       </c>
@@ -20174,7 +20174,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:14">
       <c r="A167">
         <v>161</v>
       </c>
@@ -20218,7 +20218,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:14">
       <c r="A168">
         <v>162</v>
       </c>
@@ -20262,7 +20262,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:14">
       <c r="A169">
         <v>163</v>
       </c>
@@ -20270,7 +20270,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:14">
       <c r="A170">
         <v>164</v>
       </c>
@@ -20278,7 +20278,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:14">
       <c r="A171">
         <v>165</v>
       </c>
@@ -20286,7 +20286,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:14">
       <c r="A172">
         <v>166</v>
       </c>
@@ -20294,7 +20294,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:14">
       <c r="A173">
         <v>167</v>
       </c>
@@ -20302,7 +20302,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:14">
       <c r="A174">
         <v>168</v>
       </c>
@@ -20310,7 +20310,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:14">
       <c r="A175">
         <v>169</v>
       </c>
@@ -20318,7 +20318,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:14">
       <c r="A176">
         <v>170</v>
       </c>
@@ -20326,7 +20326,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:2">
       <c r="A177">
         <v>171</v>
       </c>
@@ -20334,7 +20334,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:2">
       <c r="A178">
         <v>172</v>
       </c>
@@ -20342,7 +20342,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:2">
       <c r="A179">
         <v>173</v>
       </c>
@@ -20350,7 +20350,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:2">
       <c r="A180">
         <v>174</v>
       </c>
@@ -20358,7 +20358,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:2">
       <c r="A181">
         <v>175</v>
       </c>
@@ -20366,7 +20366,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:2">
       <c r="A182">
         <v>176</v>
       </c>
@@ -20374,7 +20374,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:2">
       <c r="A183">
         <v>177</v>
       </c>
@@ -20382,7 +20382,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:2">
       <c r="A184">
         <v>178</v>
       </c>
@@ -20390,7 +20390,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:2">
       <c r="A185">
         <v>179</v>
       </c>
@@ -20398,7 +20398,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:2">
       <c r="A186">
         <v>180</v>
       </c>
@@ -20406,7 +20406,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:2">
       <c r="A187">
         <v>181</v>
       </c>
@@ -20414,7 +20414,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:2">
       <c r="A188">
         <v>182</v>
       </c>
@@ -20422,7 +20422,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:2">
       <c r="A189">
         <v>183</v>
       </c>
@@ -20430,7 +20430,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:2">
       <c r="A190">
         <v>184</v>
       </c>
@@ -20438,7 +20438,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:2">
       <c r="A191">
         <v>185</v>
       </c>
@@ -20446,7 +20446,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:2">
       <c r="A192">
         <v>186</v>
       </c>
@@ -20454,7 +20454,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:2">
       <c r="A193">
         <v>187</v>
       </c>
@@ -20462,7 +20462,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:2">
       <c r="A194">
         <v>188</v>
       </c>
@@ -20470,7 +20470,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:2">
       <c r="A195">
         <v>189</v>
       </c>
@@ -20478,7 +20478,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:2">
       <c r="A196">
         <v>190</v>
       </c>
@@ -20486,7 +20486,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:2">
       <c r="A197">
         <v>191</v>
       </c>
@@ -20494,7 +20494,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:2">
       <c r="A198">
         <v>192</v>
       </c>
@@ -20502,7 +20502,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:2">
       <c r="A199">
         <v>193</v>
       </c>
@@ -20510,7 +20510,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:2">
       <c r="A200">
         <v>194</v>
       </c>
@@ -20518,7 +20518,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:2">
       <c r="A201">
         <v>195</v>
       </c>
@@ -20526,7 +20526,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:2">
       <c r="A202">
         <v>196</v>
       </c>
@@ -20534,7 +20534,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:2">
       <c r="A203">
         <v>197</v>
       </c>
@@ -20542,7 +20542,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:2">
       <c r="A204">
         <v>198</v>
       </c>

</xml_diff>